<commit_message>
Capitalizar autor y Uppercase Título
</commit_message>
<xml_diff>
--- a/features_and_bugs.xlsx
+++ b/features_and_bugs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Higuita\Projects\fichas-lectura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7256A77C-970B-461E-9A29-054695FB5FEF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6DF65FA5-BE7E-452D-98E6-31467FE4B798}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{3AABBBDE-8A1F-41B1-8DB4-FA01BA0CB916}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{3AABBBDE-8A1F-41B1-8DB4-FA01BA0CB916}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Feature</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>footer</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0380512-48BA-4D4B-84B4-FCE302D3D4A7}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +490,7 @@
     <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -514,8 +517,11 @@
       <c r="E2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -523,23 +529,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -547,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -555,7 +567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -563,7 +575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -571,7 +583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -579,23 +591,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -603,7 +621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -611,7 +629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -619,7 +637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Cambios generales y estilos devise
</commit_message>
<xml_diff>
--- a/features_and_bugs.xlsx
+++ b/features_and_bugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Higuita\Projects\fichas-lectura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{97C0AAE8-5A39-4721-A82E-6E6F0486F513}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6A08EDE3-EA60-48FC-94CF-FCF7E58880E3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{3AABBBDE-8A1F-41B1-8DB4-FA01BA0CB916}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Feature</t>
   </si>
@@ -481,7 +481,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,6 +528,9 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -558,6 +561,9 @@
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -566,6 +572,9 @@
       <c r="B7">
         <v>2</v>
       </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -582,6 +591,9 @@
       <c r="B9">
         <v>2</v>
       </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -634,6 +646,9 @@
       <c r="B14">
         <v>2</v>
       </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -642,6 +657,9 @@
       <c r="B15">
         <v>2</v>
       </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -677,6 +695,9 @@
       <c r="B19">
         <v>2</v>
       </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -684,6 +705,9 @@
       </c>
       <c r="B20">
         <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>